<commit_message>
Changed Serial Killer list
</commit_message>
<xml_diff>
--- a/CompleteFiles/Serial Killers - Final.xlsx
+++ b/CompleteFiles/Serial Killers - Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chirag/Desktop/Behavioral_Analysis_of_Serial_Killers__MS_Thesis/CompleteFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F875087C-E524-4A58-8B9D-DB1343928376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D7BA72-3F63-3043-A9CE-B347B596566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="1070">
   <si>
     <t>Name</t>
   </si>
@@ -3222,6 +3222,15 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=H4uT6ou_ZGw</t>
+  </si>
+  <si>
+    <t>Kip Kinkel</t>
+  </si>
+  <si>
+    <t>School Shooter</t>
+  </si>
+  <si>
+    <t>https://www.pbs.org/wgbh/pages/frontline/shows/kinkel/etc/confesst.html</t>
   </si>
 </sst>
 </file>
@@ -3286,14 +3295,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3602,22 +3611,22 @@
   <dimension ref="A1:I351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="85.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="85.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3637,27 +3646,27 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>253</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>251</v>
       </c>
@@ -3677,7 +3686,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>29</v>
       </c>
@@ -3697,7 +3706,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>343</v>
       </c>
@@ -3717,7 +3726,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>322</v>
       </c>
@@ -3737,7 +3746,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>119</v>
       </c>
@@ -3757,7 +3766,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>236</v>
       </c>
@@ -3777,7 +3786,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>154</v>
       </c>
@@ -3797,7 +3806,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>509</v>
       </c>
@@ -3817,7 +3826,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>489</v>
       </c>
@@ -3837,7 +3846,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>170</v>
       </c>
@@ -3857,7 +3866,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>63</v>
       </c>
@@ -3877,7 +3886,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>442</v>
       </c>
@@ -3897,7 +3906,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>60</v>
       </c>
@@ -3917,7 +3926,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>142</v>
       </c>
@@ -3937,7 +3946,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>341</v>
       </c>
@@ -3957,7 +3966,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>39</v>
       </c>
@@ -3977,7 +3986,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>403</v>
       </c>
@@ -3997,7 +4006,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>258</v>
       </c>
@@ -4017,7 +4026,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>247</v>
       </c>
@@ -4037,7 +4046,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>316</v>
       </c>
@@ -4057,7 +4066,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>233</v>
       </c>
@@ -4077,7 +4086,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>278</v>
       </c>
@@ -4097,7 +4106,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>129</v>
       </c>
@@ -4117,7 +4126,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>332</v>
       </c>
@@ -4137,7 +4146,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>101</v>
       </c>
@@ -4157,7 +4166,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>91</v>
       </c>
@@ -4177,7 +4186,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>371</v>
       </c>
@@ -4197,7 +4206,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>505</v>
       </c>
@@ -4217,7 +4226,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>416</v>
       </c>
@@ -4237,7 +4246,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>7</v>
       </c>
@@ -4257,7 +4266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>249</v>
       </c>
@@ -4277,7 +4286,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>47</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>243</v>
       </c>
@@ -4317,7 +4326,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>181</v>
       </c>
@@ -4337,7 +4346,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>9</v>
       </c>
@@ -4357,7 +4366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>106</v>
       </c>
@@ -4377,7 +4386,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>103</v>
       </c>
@@ -4397,7 +4406,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>110</v>
       </c>
@@ -4417,7 +4426,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>374</v>
       </c>
@@ -4437,7 +4446,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>394</v>
       </c>
@@ -4457,7 +4466,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4477,7 +4486,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>282</v>
       </c>
@@ -4497,7 +4506,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>81</v>
       </c>
@@ -4517,7 +4526,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>11</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>190</v>
       </c>
@@ -4557,7 +4566,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>319</v>
       </c>
@@ -4577,7 +4586,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>369</v>
       </c>
@@ -4597,7 +4606,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>167</v>
       </c>
@@ -4617,7 +4626,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>467</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>169</v>
       </c>
@@ -4657,7 +4666,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>384</v>
       </c>
@@ -4677,7 +4686,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>352</v>
       </c>
@@ -4697,7 +4706,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>78</v>
       </c>
@@ -4717,7 +4726,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>355</v>
       </c>
@@ -4737,7 +4746,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>18</v>
       </c>
@@ -4757,7 +4766,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>314</v>
       </c>
@@ -4777,7 +4786,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>348</v>
       </c>
@@ -4797,7 +4806,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>85</v>
       </c>
@@ -4817,7 +4826,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>79</v>
       </c>
@@ -4837,7 +4846,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>381</v>
       </c>
@@ -4857,7 +4866,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>202</v>
       </c>
@@ -4877,7 +4886,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>76</v>
       </c>
@@ -4897,7 +4906,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>99</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>409</v>
       </c>
@@ -4937,7 +4946,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>203</v>
       </c>
@@ -4957,7 +4966,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>405</v>
       </c>
@@ -4977,7 +4986,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>20</v>
       </c>
@@ -4997,7 +5006,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>164</v>
       </c>
@@ -5017,7 +5026,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>440</v>
       </c>
@@ -5037,7 +5046,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>46</v>
       </c>
@@ -5057,7 +5066,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>54</v>
       </c>
@@ -5077,7 +5086,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>525</v>
       </c>
@@ -5097,7 +5106,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>77</v>
       </c>
@@ -5117,7 +5126,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>151</v>
       </c>
@@ -5137,7 +5146,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>537</v>
       </c>
@@ -5157,7 +5166,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>307</v>
       </c>
@@ -5177,7 +5186,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>71</v>
       </c>
@@ -5197,7 +5206,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>244</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>120</v>
       </c>
@@ -5237,7 +5246,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>148</v>
       </c>
@@ -5260,7 +5269,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>17</v>
       </c>
@@ -5280,7 +5289,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>192</v>
       </c>
@@ -5300,7 +5309,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>105</v>
       </c>
@@ -5320,7 +5329,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>360</v>
       </c>
@@ -5340,7 +5349,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>521</v>
       </c>
@@ -5360,7 +5369,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>558</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>123</v>
       </c>
@@ -5400,7 +5409,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>383</v>
       </c>
@@ -5420,7 +5429,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>178</v>
       </c>
@@ -5440,7 +5449,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>182</v>
       </c>
@@ -5460,7 +5469,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>88</v>
       </c>
@@ -5480,7 +5489,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>413</v>
       </c>
@@ -5500,7 +5509,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>68</v>
       </c>
@@ -5520,7 +5529,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>479</v>
       </c>
@@ -5540,7 +5549,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>480</v>
       </c>
@@ -5560,7 +5569,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>23</v>
       </c>
@@ -5580,7 +5589,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>94</v>
       </c>
@@ -5600,7 +5609,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>379</v>
       </c>
@@ -5620,7 +5629,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>59</v>
       </c>
@@ -5640,7 +5649,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>134</v>
       </c>
@@ -5660,7 +5669,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>72</v>
       </c>
@@ -5680,7 +5689,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>0</v>
       </c>
@@ -5700,7 +5709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>242</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>227</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>283</v>
       </c>
@@ -5760,7 +5769,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>214</v>
       </c>
@@ -5780,7 +5789,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>53</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>538</v>
       </c>
@@ -5820,7 +5829,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>268</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>96</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>82</v>
       </c>
@@ -5880,7 +5889,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>141</v>
       </c>
@@ -5900,7 +5909,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>408</v>
       </c>
@@ -5920,7 +5929,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>62</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>56</v>
       </c>
@@ -5960,7 +5969,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>281</v>
       </c>
@@ -5980,7 +5989,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>255</v>
       </c>
@@ -6000,7 +6009,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>531</v>
       </c>
@@ -6020,7 +6029,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>545</v>
       </c>
@@ -6040,7 +6049,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>8</v>
       </c>
@@ -6060,7 +6069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>200</v>
       </c>
@@ -6080,7 +6089,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>495</v>
       </c>
@@ -6100,7 +6109,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>168</v>
       </c>
@@ -6120,7 +6129,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>544</v>
       </c>
@@ -6140,7 +6149,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>425</v>
       </c>
@@ -6160,7 +6169,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>175</v>
       </c>
@@ -6180,7 +6189,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>388</v>
       </c>
@@ -6200,7 +6209,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>5</v>
       </c>
@@ -6220,7 +6229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>177</v>
       </c>
@@ -6240,7 +6249,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>392</v>
       </c>
@@ -6260,7 +6269,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>199</v>
       </c>
@@ -6280,7 +6289,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>12</v>
       </c>
@@ -6300,7 +6309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>40</v>
       </c>
@@ -6320,7 +6329,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>198</v>
       </c>
@@ -6340,7 +6349,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>34</v>
       </c>
@@ -6360,7 +6369,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>424</v>
       </c>
@@ -6380,7 +6389,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>97</v>
       </c>
@@ -6400,7 +6409,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>296</v>
       </c>
@@ -6420,7 +6429,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>157</v>
       </c>
@@ -6440,7 +6449,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>396</v>
       </c>
@@ -6460,7 +6469,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>235</v>
       </c>
@@ -6480,7 +6489,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>496</v>
       </c>
@@ -6500,7 +6509,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>28</v>
       </c>
@@ -6520,7 +6529,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>402</v>
       </c>
@@ -6540,7 +6549,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>476</v>
       </c>
@@ -6569,7 +6578,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>391</v>
       </c>
@@ -6589,7 +6598,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>419</v>
       </c>
@@ -6609,7 +6618,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>447</v>
       </c>
@@ -6629,7 +6638,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>172</v>
       </c>
@@ -6649,7 +6658,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>367</v>
       </c>
@@ -6669,7 +6678,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>201</v>
       </c>
@@ -6689,7 +6698,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>366</v>
       </c>
@@ -6709,7 +6718,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>475</v>
       </c>
@@ -6729,7 +6738,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>549</v>
       </c>
@@ -6749,7 +6758,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>327</v>
       </c>
@@ -6769,7 +6778,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>329</v>
       </c>
@@ -6789,7 +6798,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>354</v>
       </c>
@@ -6809,7 +6818,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>93</v>
       </c>
@@ -6829,7 +6838,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>293</v>
       </c>
@@ -6849,7 +6858,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1</v>
       </c>
@@ -6869,7 +6878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>138</v>
       </c>
@@ -6889,7 +6898,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>260</v>
       </c>
@@ -6909,7 +6918,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>30</v>
       </c>
@@ -6929,7 +6938,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>517</v>
       </c>
@@ -6949,7 +6958,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>188</v>
       </c>
@@ -6969,7 +6978,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>468</v>
       </c>
@@ -6989,7 +6998,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>528</v>
       </c>
@@ -7009,7 +7018,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>83</v>
       </c>
@@ -7029,7 +7038,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>183</v>
       </c>
@@ -7049,7 +7058,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>265</v>
       </c>
@@ -7069,7 +7078,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>32</v>
       </c>
@@ -7089,7 +7098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>238</v>
       </c>
@@ -7109,7 +7118,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>491</v>
       </c>
@@ -7129,7 +7138,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>41</v>
       </c>
@@ -7149,7 +7158,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>536</v>
       </c>
@@ -7169,7 +7178,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>131</v>
       </c>
@@ -7189,7 +7198,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>370</v>
       </c>
@@ -7209,7 +7218,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>237</v>
       </c>
@@ -7229,7 +7238,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>166</v>
       </c>
@@ -7249,7 +7258,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>250</v>
       </c>
@@ -7269,7 +7278,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>35</v>
       </c>
@@ -7289,7 +7298,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>483</v>
       </c>
@@ -7309,7 +7318,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>89</v>
       </c>
@@ -7329,7 +7338,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>378</v>
       </c>
@@ -7349,7 +7358,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>498</v>
       </c>
@@ -7369,7 +7378,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>429</v>
       </c>
@@ -7389,7 +7398,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>263</v>
       </c>
@@ -7409,7 +7418,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>443</v>
       </c>
@@ -7429,7 +7438,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>80</v>
       </c>
@@ -7449,7 +7458,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>26</v>
       </c>
@@ -7469,7 +7478,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>430</v>
       </c>
@@ -7489,7 +7498,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>259</v>
       </c>
@@ -7509,7 +7518,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>173</v>
       </c>
@@ -7529,7 +7538,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>191</v>
       </c>
@@ -7549,7 +7558,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>484</v>
       </c>
@@ -7569,7 +7578,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>439</v>
       </c>
@@ -7589,7 +7598,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>43</v>
       </c>
@@ -7609,7 +7618,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>435</v>
       </c>
@@ -7629,7 +7638,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>186</v>
       </c>
@@ -7649,7 +7658,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>415</v>
       </c>
@@ -7669,7 +7678,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>446</v>
       </c>
@@ -7689,7 +7698,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>69</v>
       </c>
@@ -7709,7 +7718,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>239</v>
       </c>
@@ -7729,7 +7738,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>513</v>
       </c>
@@ -7749,7 +7758,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>209</v>
       </c>
@@ -7769,7 +7778,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>143</v>
       </c>
@@ -7789,7 +7798,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>25</v>
       </c>
@@ -7809,7 +7818,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>445</v>
       </c>
@@ -7829,7 +7838,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>16</v>
       </c>
@@ -7849,7 +7858,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>228</v>
       </c>
@@ -7869,7 +7878,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>410</v>
       </c>
@@ -7889,7 +7898,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>458</v>
       </c>
@@ -7909,7 +7918,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>13</v>
       </c>
@@ -7929,7 +7938,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>111</v>
       </c>
@@ -7949,7 +7958,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>205</v>
       </c>
@@ -7969,7 +7978,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>492</v>
       </c>
@@ -7989,7 +7998,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>326</v>
       </c>
@@ -8009,7 +8018,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>423</v>
       </c>
@@ -8029,7 +8038,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>426</v>
       </c>
@@ -8049,7 +8058,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>21</v>
       </c>
@@ -8069,7 +8078,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>556</v>
       </c>
@@ -8089,7 +8098,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>102</v>
       </c>
@@ -8109,7 +8118,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>433</v>
       </c>
@@ -8129,7 +8138,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>133</v>
       </c>
@@ -8149,7 +8158,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>4</v>
       </c>
@@ -8169,7 +8178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>428</v>
       </c>
@@ -8189,7 +8198,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>534</v>
       </c>
@@ -8209,7 +8218,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>299</v>
       </c>
@@ -8229,7 +8238,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>180</v>
       </c>
@@ -8249,7 +8258,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>137</v>
       </c>
@@ -8269,7 +8278,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>362</v>
       </c>
@@ -8289,7 +8298,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>75</v>
       </c>
@@ -8309,7 +8318,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>122</v>
       </c>
@@ -8329,7 +8338,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>147</v>
       </c>
@@ -8349,7 +8358,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>279</v>
       </c>
@@ -8369,7 +8378,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>376</v>
       </c>
@@ -8389,7 +8398,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>551</v>
       </c>
@@ -8409,7 +8418,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>31</v>
       </c>
@@ -8429,7 +8438,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>274</v>
       </c>
@@ -8449,7 +8458,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>418</v>
       </c>
@@ -8469,7 +8478,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>399</v>
       </c>
@@ -8489,7 +8498,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>184</v>
       </c>
@@ -8509,7 +8518,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>547</v>
       </c>
@@ -8529,7 +8538,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>87</v>
       </c>
@@ -8549,7 +8558,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>490</v>
       </c>
@@ -8569,7 +8578,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>320</v>
       </c>
@@ -8589,7 +8598,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>375</v>
       </c>
@@ -8609,7 +8618,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>313</v>
       </c>
@@ -8629,7 +8638,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>223</v>
       </c>
@@ -8649,7 +8658,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>145</v>
       </c>
@@ -8669,7 +8678,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>222</v>
       </c>
@@ -8689,7 +8698,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>204</v>
       </c>
@@ -8709,7 +8718,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>109</v>
       </c>
@@ -8729,7 +8738,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>55</v>
       </c>
@@ -8749,7 +8758,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>262</v>
       </c>
@@ -8769,7 +8778,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>414</v>
       </c>
@@ -8789,7 +8798,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>10</v>
       </c>
@@ -8809,7 +8818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>315</v>
       </c>
@@ -8829,7 +8838,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>482</v>
       </c>
@@ -8849,7 +8858,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>27</v>
       </c>
@@ -8869,7 +8878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>36</v>
       </c>
@@ -8889,7 +8898,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>146</v>
       </c>
@@ -8909,7 +8918,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>493</v>
       </c>
@@ -8929,7 +8938,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>516</v>
       </c>
@@ -8949,7 +8958,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>380</v>
       </c>
@@ -8969,7 +8978,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>364</v>
       </c>
@@ -8989,7 +8998,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>292</v>
       </c>
@@ -9009,7 +9018,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>411</v>
       </c>
@@ -9029,7 +9038,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>555</v>
       </c>
@@ -9049,7 +9058,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>124</v>
       </c>
@@ -9069,7 +9078,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>33</v>
       </c>
@@ -9089,7 +9098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>65</v>
       </c>
@@ -9109,7 +9118,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>2</v>
       </c>
@@ -9129,7 +9138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>261</v>
       </c>
@@ -9149,7 +9158,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>264</v>
       </c>
@@ -9169,7 +9178,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>257</v>
       </c>
@@ -9189,7 +9198,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>189</v>
       </c>
@@ -9209,7 +9218,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>245</v>
       </c>
@@ -9229,7 +9238,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>284</v>
       </c>
@@ -9249,7 +9258,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>73</v>
       </c>
@@ -9269,7 +9278,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>560</v>
       </c>
@@ -9289,7 +9298,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>179</v>
       </c>
@@ -9309,7 +9318,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>225</v>
       </c>
@@ -9329,7 +9338,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>338</v>
       </c>
@@ -9349,7 +9358,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>478</v>
       </c>
@@ -9369,7 +9378,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>273</v>
       </c>
@@ -9389,7 +9398,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>365</v>
       </c>
@@ -9409,7 +9418,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>404</v>
       </c>
@@ -9429,7 +9438,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>108</v>
       </c>
@@ -9449,7 +9458,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>176</v>
       </c>
@@ -9469,7 +9478,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>165</v>
       </c>
@@ -9489,7 +9498,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>540</v>
       </c>
@@ -9509,7 +9518,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>431</v>
       </c>
@@ -9529,7 +9538,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>363</v>
       </c>
@@ -9549,7 +9558,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>19</v>
       </c>
@@ -9569,7 +9578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>229</v>
       </c>
@@ -9589,7 +9598,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>497</v>
       </c>
@@ -9609,7 +9618,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>450</v>
       </c>
@@ -9629,7 +9638,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>412</v>
       </c>
@@ -9649,7 +9658,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>303</v>
       </c>
@@ -9669,7 +9678,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>309</v>
       </c>
@@ -9689,7 +9698,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>486</v>
       </c>
@@ -9709,7 +9718,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>107</v>
       </c>
@@ -9729,7 +9738,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>393</v>
       </c>
@@ -9749,7 +9758,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>67</v>
       </c>
@@ -9769,7 +9778,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>127</v>
       </c>
@@ -9789,7 +9798,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>240</v>
       </c>
@@ -9809,7 +9818,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>290</v>
       </c>
@@ -9829,7 +9838,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>294</v>
       </c>
@@ -9849,7 +9858,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>136</v>
       </c>
@@ -9869,7 +9878,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>308</v>
       </c>
@@ -9889,7 +9898,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>524</v>
       </c>
@@ -9909,7 +9918,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>125</v>
       </c>
@@ -9929,7 +9938,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>395</v>
       </c>
@@ -9949,7 +9958,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>66</v>
       </c>
@@ -9969,7 +9978,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>449</v>
       </c>
@@ -9989,7 +9998,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>331</v>
       </c>
@@ -10009,7 +10018,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>422</v>
       </c>
@@ -10029,7 +10038,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>187</v>
       </c>
@@ -10049,7 +10058,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>197</v>
       </c>
@@ -10069,7 +10078,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>508</v>
       </c>
@@ -10089,7 +10098,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>347</v>
       </c>
@@ -10109,7 +10118,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>436</v>
       </c>
@@ -10129,7 +10138,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>37</v>
       </c>
@@ -10149,7 +10158,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>317</v>
       </c>
@@ -10169,7 +10178,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>421</v>
       </c>
@@ -10189,7 +10198,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>213</v>
       </c>
@@ -10209,7 +10218,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>291</v>
       </c>
@@ -10229,7 +10238,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>248</v>
       </c>
@@ -10249,7 +10258,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>252</v>
       </c>
@@ -10269,7 +10278,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>22</v>
       </c>
@@ -10289,7 +10298,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>427</v>
       </c>
@@ -10309,7 +10318,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>453</v>
       </c>
@@ -10329,7 +10338,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>163</v>
       </c>
@@ -10349,7 +10358,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>417</v>
       </c>
@@ -10369,7 +10378,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>185</v>
       </c>
@@ -10389,7 +10398,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>206</v>
       </c>
@@ -10409,7 +10418,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>448</v>
       </c>
@@ -10429,7 +10438,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>92</v>
       </c>
@@ -10449,7 +10458,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>45</v>
       </c>
@@ -10469,7 +10478,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>444</v>
       </c>
@@ -10489,7 +10498,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>437</v>
       </c>
@@ -10509,7 +10518,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>288</v>
       </c>
@@ -10529,7 +10538,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>57</v>
       </c>
@@ -10549,7 +10558,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>90</v>
       </c>
@@ -10569,7 +10578,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>3</v>
       </c>
@@ -10589,7 +10598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>194</v>
       </c>
@@ -10609,7 +10618,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>523</v>
       </c>
@@ -10629,7 +10638,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>70</v>
       </c>
@@ -10665,19 +10674,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85718300-C945-42BC-A552-D67A75D2D7B2}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="43.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1034</v>
       </c>
@@ -10685,30 +10695,30 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>1036</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
       <c r="C4" s="4" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
       <c r="C5" s="4" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>1040</v>
       </c>
@@ -10716,7 +10726,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1042</v>
       </c>
@@ -10724,92 +10734,103 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>1047</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>1055</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>1058</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>1059</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>1063</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>1065</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>1066</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>1069</v>
       </c>
     </row>
   </sheetData>
@@ -10825,8 +10846,9 @@
     <hyperlink ref="C9" r:id="rId6" xr:uid="{7C592F0E-4B93-4D23-9E33-09E8A0F3E564}"/>
     <hyperlink ref="C23" r:id="rId7" xr:uid="{8009615A-BA4F-430D-B211-5D085FC3E37B}"/>
     <hyperlink ref="C24" r:id="rId8" xr:uid="{C93290F0-0622-4B3B-877D-AC9524CFB78B}"/>
+    <hyperlink ref="C28" r:id="rId9" xr:uid="{4DA8E5BE-2C13-384F-A36A-2BC2E1C6E7B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new data sources.
</commit_message>
<xml_diff>
--- a/CompleteFiles/Serial Killers - Final.xlsx
+++ b/CompleteFiles/Serial Killers - Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chirag/Desktop/Behavioral_Analysis_of_Serial_Killers__MS_Thesis/CompleteFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D7BA72-3F63-3043-A9CE-B347B596566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1133B1F-9177-4A40-B1C2-04A0972FA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1075">
   <si>
     <t>Name</t>
   </si>
@@ -3231,6 +3231,21 @@
   </si>
   <si>
     <t>https://www.pbs.org/wgbh/pages/frontline/shows/kinkel/etc/confesst.html</t>
+  </si>
+  <si>
+    <t>Aileen Wuornos letter to close friend Dawn Boydkins regarding the movie “Monster”</t>
+  </si>
+  <si>
+    <t>Jeffrey Dahmer's Last Interview</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sm6yAnov4O8&amp;list=PLPtSw9ajDwcSSUT0PBTJotR0z7Au39EBP&amp;index=2&amp;ab_channel=TrueCrimeMagazine</t>
+  </si>
+  <si>
+    <t>Serial Killers Interview Playlist</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLPtSw9ajDwcSSUT0PBTJotR0z7Au39EBP</t>
   </si>
 </sst>
 </file>
@@ -3283,7 +3298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3302,6 +3317,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10674,10 +10692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85718300-C945-42BC-A552-D67A75D2D7B2}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10831,6 +10849,27 @@
       </c>
       <c r="C28" s="4" t="s">
         <v>1069</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>1074</v>
       </c>
     </row>
   </sheetData>
@@ -10847,8 +10886,10 @@
     <hyperlink ref="C23" r:id="rId7" xr:uid="{8009615A-BA4F-430D-B211-5D085FC3E37B}"/>
     <hyperlink ref="C24" r:id="rId8" xr:uid="{C93290F0-0622-4B3B-877D-AC9524CFB78B}"/>
     <hyperlink ref="C28" r:id="rId9" xr:uid="{4DA8E5BE-2C13-384F-A36A-2BC2E1C6E7B3}"/>
+    <hyperlink ref="C33" r:id="rId10" xr:uid="{2F4FAC23-18F4-5143-A620-499B4226A3C2}"/>
+    <hyperlink ref="C35" r:id="rId11" xr:uid="{DA807762-CAD8-AC45-B10E-E3097FC74C8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added code to work on a test interview data
</commit_message>
<xml_diff>
--- a/CompleteFiles/Serial Killers - Final.xlsx
+++ b/CompleteFiles/Serial Killers - Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chirag/Desktop/Behavioral_Analysis_of_Serial_Killers__MS_Thesis/CompleteFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1133B1F-9177-4A40-B1C2-04A0972FA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF266EB0-2320-DD42-A7E6-1A8BD50887F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -3263,6 +3263,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3316,10 +3317,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10694,8 +10695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85718300-C945-42BC-A552-D67A75D2D7B2}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10717,7 +10718,7 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>1036</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -10725,13 +10726,13 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="C4" s="4" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="C5" s="4" t="s">
         <v>1039</v>
       </c>
@@ -10852,7 +10853,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>1070</v>
       </c>
     </row>

</xml_diff>